<commit_message>
Test Working. Going to start study session
</commit_message>
<xml_diff>
--- a/Documents/DB Design/AfterUG-DB-v1.1.xlsx
+++ b/Documents/DB Design/AfterUG-DB-v1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\AfterUG\Code\afterug\Documents\DB Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\code-git\afterug-git-latest\Documents\DB Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -595,7 +595,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
   <si>
     <t>QuestionType</t>
   </si>
@@ -847,6 +847,39 @@
   </si>
   <si>
     <t>UserWhoRatedDifficultyID</t>
+  </si>
+  <si>
+    <t>NoOfQuestionsPerTest</t>
+  </si>
+  <si>
+    <t>NoOfChoicesPerQuestion</t>
+  </si>
+  <si>
+    <t>GlobalSettings</t>
+  </si>
+  <si>
+    <t>GlobalSettingsID</t>
+  </si>
+  <si>
+    <t>NoOfRepetitionsIncorrect</t>
+  </si>
+  <si>
+    <t>NoOfRepetitionsCorrect</t>
+  </si>
+  <si>
+    <t>UserSettings</t>
+  </si>
+  <si>
+    <t>UserSettingsID</t>
+  </si>
+  <si>
+    <t>NoOfQuestionsForWeeklyReview</t>
+  </si>
+  <si>
+    <t>NoOfChoicesForWeeklyReview</t>
+  </si>
+  <si>
+    <t>Etc add what ever comes to mind</t>
   </si>
 </sst>
 </file>
@@ -1318,14 +1351,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
@@ -1697,34 +1730,90 @@
         <v>14</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Wordlist and GK Working Properly. Good Stable version
</commit_message>
<xml_diff>
--- a/Documents/DB Design/AfterUG-DB-v1.1.xlsx
+++ b/Documents/DB Design/AfterUG-DB-v1.1.xlsx
@@ -172,30 +172,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>AfterUGNotePointsTags Table</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F6" authorId="0" shapeId="0">
       <text>
         <r>
@@ -577,6 +553,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="D27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>computer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If not yet prpoved by user show the expalanation for the user who added that. If approved show userexplanation after AUG
+explanation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A38" authorId="0" shapeId="0">
       <text>
         <r>
@@ -595,7 +596,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
   <si>
     <t>QuestionType</t>
   </si>
@@ -723,9 +724,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>AfterUGNotePointText</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -880,6 +878,48 @@
   </si>
   <si>
     <t>Etc add what ever comes to mind</t>
+  </si>
+  <si>
+    <t>AUGNotesAddedByEmployeeUser</t>
+  </si>
+  <si>
+    <t>AUGNotesApprovedByEmployeeUser</t>
+  </si>
+  <si>
+    <t>AUGNotes</t>
+  </si>
+  <si>
+    <t>AUGNotesID</t>
+  </si>
+  <si>
+    <t>AUGNotePointText</t>
+  </si>
+  <si>
+    <t>ExplanationText</t>
+  </si>
+  <si>
+    <t>AddedByUserID</t>
+  </si>
+  <si>
+    <t>ApprovedByUserID</t>
+  </si>
+  <si>
+    <t>UserExplanationID</t>
+  </si>
+  <si>
+    <t>AUGExplanationID</t>
+  </si>
+  <si>
+    <t>UserChoiceExplanation</t>
+  </si>
+  <si>
+    <t>AUGChoiceExplanation</t>
+  </si>
+  <si>
+    <t>QuestionExplanation</t>
+  </si>
+  <si>
+    <t>QuestionExplanationID</t>
   </si>
 </sst>
 </file>
@@ -1351,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,9 +1401,8 @@
     <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
@@ -1378,13 +1417,13 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>22</v>
@@ -1399,10 +1438,10 @@
         <v>31</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1416,10 +1455,10 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1437,7 +1476,7 @@
         <v>36</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1460,7 +1499,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>16</v>
@@ -1472,7 +1511,7 @@
         <v>38</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1486,10 +1525,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>16</v>
@@ -1518,7 +1557,10 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -1535,10 +1577,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
       </c>
       <c r="F6" t="s">
         <v>40</v>
@@ -1547,7 +1589,7 @@
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1555,7 +1597,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1566,7 +1611,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1574,43 +1619,43 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1618,25 +1663,25 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1650,7 +1695,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>15</v>
@@ -1676,19 +1721,19 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1696,134 +1741,188 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -1833,12 +1932,12 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>